<commit_message>
update sprint or whatever
yes
</commit_message>
<xml_diff>
--- a/semaine_13/Feuille_de_temps_S1-Eq2.xlsx
+++ b/semaine_13/Feuille_de_temps_S1-Eq2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Denis\OneDrive - Collège de Bois-de-Boulogne\Bureau\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\2281126\Documents\GitHub\CoolKidsClub-Gym\semaine_13\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E56977D-5B04-44B6-B095-78B794A90627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13368672-AE17-4801-8E81-E2F988C521E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="326" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32265" yWindow="3465" windowWidth="21600" windowHeight="11385" tabRatio="326" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="118">
   <si>
     <t>Temps</t>
   </si>
@@ -388,6 +388,12 @@
   </si>
   <si>
     <t>Tenter de faire Appliquer</t>
+  </si>
+  <si>
+    <t>coder review collection</t>
+  </si>
+  <si>
+    <t>coder abonnement collection</t>
   </si>
 </sst>
 </file>
@@ -547,7 +553,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -852,7 +858,7 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -1068,7 +1074,7 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="40.28515625" customWidth="1"/>
     <col min="4" max="4" width="26.7109375" customWidth="1"/>
@@ -1202,11 +1208,11 @@
   </sheetPr>
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -8417,7 +8423,7 @@
       <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
   </cols>
@@ -8679,11 +8685,11 @@
   </sheetPr>
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
@@ -8812,6 +8818,12 @@
       <c r="V2" t="s">
         <v>110</v>
       </c>
+      <c r="W2">
+        <v>2</v>
+      </c>
+      <c r="X2" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -8843,6 +8855,12 @@
       </c>
       <c r="L3" t="s">
         <v>107</v>
+      </c>
+      <c r="W3">
+        <v>1.5</v>
+      </c>
+      <c r="X3" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8854,6 +8872,12 @@
       <c r="F4" t="s">
         <v>103</v>
       </c>
+      <c r="W4">
+        <v>2</v>
+      </c>
+      <c r="X4" t="s">
+        <v>107</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>